<commit_message>
fix createdAt mockup data
</commit_message>
<xml_diff>
--- a/src/models/data/patient.xlsx
+++ b/src/models/data/patient.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Hoc_Ki_VIII\src\MEDRE_BE\src\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C412735-4C8A-4107-890C-D8FC0037D577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606F1524-1392-4887-B715-949D84E98843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="19224" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="141">
   <si>
     <t>phone_number</t>
   </si>
@@ -396,6 +396,69 @@
   </si>
   <si>
     <t>0564461389</t>
+  </si>
+  <si>
+    <t>createdAt</t>
+  </si>
+  <si>
+    <t>updatedAt</t>
+  </si>
+  <si>
+    <t>2023-04-16T03:42:46.836Z</t>
+  </si>
+  <si>
+    <t>2023-04-09T03:20:31.077Z</t>
+  </si>
+  <si>
+    <t>2023-04-19T12:32:13.787Z</t>
+  </si>
+  <si>
+    <t>2023-04-20T18:59:51.241Z</t>
+  </si>
+  <si>
+    <t>2023-04-12T20:57:30.058Z</t>
+  </si>
+  <si>
+    <t>2023-04-18T13:51:56.194Z</t>
+  </si>
+  <si>
+    <t>2023-04-20T02:09:40.846Z</t>
+  </si>
+  <si>
+    <t>2023-04-21T01:45:38.618Z</t>
+  </si>
+  <si>
+    <t>2023-04-23T04:44:42.471Z</t>
+  </si>
+  <si>
+    <t>2023-05-02T13:49:47.409Z</t>
+  </si>
+  <si>
+    <t>2023-05-02T10:13:51.564Z</t>
+  </si>
+  <si>
+    <t>2023-05-03T12:04:43.165Z</t>
+  </si>
+  <si>
+    <t>2023-05-02T12:12:13.632Z</t>
+  </si>
+  <si>
+    <t>2023-05-16T18:31:08.185Z</t>
+  </si>
+  <si>
+    <t>2023-05-08T08:54:59.583Z</t>
+  </si>
+  <si>
+    <t>2023-05-07T11:40:13.109Z</t>
+  </si>
+  <si>
+    <t>2023-05-08T12:27:27.314Z</t>
+  </si>
+  <si>
+    <t>2023-05-10T21:47:27.523Z</t>
+  </si>
+  <si>
+    <t>2023-05-09T04:25:04.137Z</t>
   </si>
 </sst>
 </file>
@@ -728,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,9 +805,10 @@
     <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.77734375" customWidth="1"/>
+    <col min="8" max="9" width="23.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -766,8 +830,14 @@
       <c r="G1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -789,8 +859,14 @@
       <c r="G2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -812,8 +888,14 @@
       <c r="G3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -835,8 +917,14 @@
       <c r="G4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -858,8 +946,14 @@
       <c r="G5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -881,8 +975,14 @@
       <c r="G6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -904,8 +1004,14 @@
       <c r="G7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>103</v>
       </c>
@@ -927,8 +1033,14 @@
       <c r="G8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>128</v>
+      </c>
+      <c r="I8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>115</v>
       </c>
@@ -950,8 +1062,14 @@
       <c r="G9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -973,8 +1091,14 @@
       <c r="G10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>109</v>
       </c>
@@ -996,8 +1120,14 @@
       <c r="G11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>131</v>
+      </c>
+      <c r="I11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>104</v>
       </c>
@@ -1019,8 +1149,14 @@
       <c r="G12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>101</v>
       </c>
@@ -1042,8 +1178,14 @@
       <c r="G13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>111</v>
       </c>
@@ -1065,8 +1207,14 @@
       <c r="G14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>134</v>
+      </c>
+      <c r="I14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>102</v>
       </c>
@@ -1088,8 +1236,14 @@
       <c r="G15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>135</v>
+      </c>
+      <c r="I15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>113</v>
       </c>
@@ -1111,8 +1265,14 @@
       <c r="G16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>136</v>
+      </c>
+      <c r="I16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>105</v>
       </c>
@@ -1134,8 +1294,14 @@
       <c r="G17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>137</v>
+      </c>
+      <c r="I17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -1157,8 +1323,14 @@
       <c r="G18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>138</v>
+      </c>
+      <c r="I18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -1180,8 +1352,14 @@
       <c r="G19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>139</v>
+      </c>
+      <c r="I19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>106</v>
       </c>
@@ -1202,6 +1380,12 @@
       </c>
       <c r="G20" t="s">
         <v>29</v>
+      </c>
+      <c r="H20" t="s">
+        <v>140</v>
+      </c>
+      <c r="I20" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>